<commit_message>
Updates to job.ini files and bash scripts
</commit_message>
<xml_diff>
--- a/model-scripts/model-parameters_.xlsx
+++ b/model-scripts/model-parameters_.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/murrayjourneay/OpenDRR/canada-srm2/model-scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjournea\OpenDRR\canada-srm2\model-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1D5FBB-D893-4E43-9930-BA937633A851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="46480" windowHeight="22180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="46485" windowHeight="22185" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="srm-regions" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="srm-parameters" sheetId="3" r:id="rId3"/>
     <sheet name="srm-exports" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1622,12 +1621,6 @@
     <t>eD_[region]_sources.csv</t>
   </si>
   <si>
-    <t>dmg_by_asset</t>
-  </si>
-  <si>
-    <t>eD_[region]_dmg_by_asset_[b0,r2].csv</t>
-  </si>
-  <si>
     <t>consequences.py</t>
   </si>
   <si>
@@ -1659,13 +1652,19 @@
   </si>
   <si>
     <t>ebR_[region]_agg_losses-stats_[b0,r2].csv</t>
+  </si>
+  <si>
+    <t>eD_[region]_damages-meant_[b0,r2].csv</t>
+  </si>
+  <si>
+    <t>avg-damages-mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -3146,7 +3145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3156,21 +3155,21 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="102" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="16.33203125" style="1"/>
+    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3196,7 +3195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="20.25" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="20.25" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -3274,7 +3273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="20.25" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -3300,7 +3299,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="20.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="20.25" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="20.25" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -3378,7 +3377,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="20.25" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
@@ -3404,7 +3403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="20.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
@@ -3430,7 +3429,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="20.25" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="20.25" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
@@ -3482,7 +3481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="20.25" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="20.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
@@ -3534,7 +3533,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="20.25" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="20.25" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
@@ -3586,7 +3585,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="20.25" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>47</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="20.25" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>49</v>
       </c>
@@ -3638,7 +3637,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="20.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>51</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="20.25" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>51</v>
       </c>
@@ -3690,7 +3689,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" ht="20.25" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>51</v>
       </c>
@@ -3716,7 +3715,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="20.25" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>51</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="20.25" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>51</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="20.25" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>51</v>
       </c>
@@ -3794,7 +3793,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="20.25" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>51</v>
       </c>
@@ -3820,7 +3819,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="20.25" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" ht="20.25" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="20.25" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>71</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="20.25" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>73</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="20.25" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>73</v>
       </c>
@@ -3950,7 +3949,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="20.25" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>73</v>
       </c>
@@ -3976,7 +3975,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="20.25" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>73</v>
       </c>
@@ -4002,7 +4001,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="20.25" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>73</v>
       </c>
@@ -4028,7 +4027,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="20.25" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>73</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="20.25" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>73</v>
       </c>
@@ -4080,7 +4079,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" ht="20.25" customHeight="1">
       <c r="A36" s="10" t="s">
         <v>89</v>
       </c>
@@ -4106,7 +4105,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" ht="20.25" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>89</v>
       </c>
@@ -4132,7 +4131,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="20.25" customHeight="1">
       <c r="A38" s="10" t="s">
         <v>95</v>
       </c>
@@ -4168,7 +4167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4178,22 +4177,22 @@
       <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="14.33203125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="19" customWidth="1"/>
+    <col min="1" max="2" width="14.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="19" customWidth="1"/>
     <col min="4" max="4" width="15" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="19" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="19" customWidth="1"/>
     <col min="8" max="8" width="25" style="19" customWidth="1"/>
     <col min="9" max="10" width="29" style="19" customWidth="1"/>
-    <col min="11" max="12" width="25.83203125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="19" customWidth="1"/>
-    <col min="14" max="16384" width="16.33203125" style="19"/>
+    <col min="11" max="12" width="25.85546875" style="19" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="19" customWidth="1"/>
+    <col min="14" max="16384" width="16.28515625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="20.45" customHeight="1">
       <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4254,7 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
     </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="20.25" customHeight="1">
       <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="20.25" customHeight="1">
       <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="20.25" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="A6" s="22" t="s">
         <v>8</v>
       </c>
@@ -4383,7 +4382,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="20.25" customHeight="1">
       <c r="A7" s="22" t="s">
         <v>8</v>
       </c>
@@ -4415,7 +4414,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="20.25" customHeight="1">
       <c r="A8" s="22" t="s">
         <v>20</v>
       </c>
@@ -4441,7 +4440,7 @@
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
     </row>
-    <row r="9" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="20.25" customHeight="1">
       <c r="A9" s="22" t="s">
         <v>20</v>
       </c>
@@ -4475,7 +4474,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="20.25" customHeight="1">
       <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
@@ -4509,7 +4508,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="20.25" customHeight="1">
       <c r="A11" s="22" t="s">
         <v>20</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="20.25" customHeight="1">
       <c r="A12" s="22" t="s">
         <v>20</v>
       </c>
@@ -4577,7 +4576,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="20.25" customHeight="1">
       <c r="A13" s="22" t="s">
         <v>20</v>
       </c>
@@ -4611,7 +4610,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="20.25" customHeight="1">
       <c r="A14" s="22" t="s">
         <v>32</v>
       </c>
@@ -4635,7 +4634,7 @@
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
     </row>
-    <row r="15" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="20.25" customHeight="1">
       <c r="A15" s="22" t="s">
         <v>32</v>
       </c>
@@ -4667,7 +4666,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="20.25" customHeight="1">
       <c r="A16" s="22" t="s">
         <v>32</v>
       </c>
@@ -4699,7 +4698,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="20.25" customHeight="1">
       <c r="A17" s="22" t="s">
         <v>38</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="20.25" customHeight="1">
       <c r="A18" s="22" t="s">
         <v>41</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="20.25" customHeight="1">
       <c r="A19" s="22" t="s">
         <v>44</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="20.25" customHeight="1">
       <c r="A20" s="22" t="s">
         <v>47</v>
       </c>
@@ -4843,7 +4842,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" ht="20.25" customHeight="1">
       <c r="A21" s="22" t="s">
         <v>49</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" ht="20.25" customHeight="1">
       <c r="A22" s="22" t="s">
         <v>51</v>
       </c>
@@ -4903,7 +4902,7 @@
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
     </row>
-    <row r="23" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" ht="20.25" customHeight="1">
       <c r="A23" s="22" t="s">
         <v>51</v>
       </c>
@@ -4935,7 +4934,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" ht="20.25" customHeight="1">
       <c r="A24" s="22" t="s">
         <v>51</v>
       </c>
@@ -4967,7 +4966,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" ht="20.25" customHeight="1">
       <c r="A25" s="22" t="s">
         <v>51</v>
       </c>
@@ -4999,7 +4998,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" ht="20.25" customHeight="1">
       <c r="A26" s="22" t="s">
         <v>51</v>
       </c>
@@ -5031,7 +5030,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" ht="20.25" customHeight="1">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" ht="20.25" customHeight="1">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" ht="20.25" customHeight="1">
       <c r="A29" s="22" t="s">
         <v>51</v>
       </c>
@@ -5127,7 +5126,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" ht="20.25" customHeight="1">
       <c r="A30" s="22" t="s">
         <v>51</v>
       </c>
@@ -5159,7 +5158,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" ht="20.25" customHeight="1">
       <c r="A31" s="22" t="s">
         <v>51</v>
       </c>
@@ -5191,7 +5190,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" ht="20.25" customHeight="1">
       <c r="A32" s="22" t="s">
         <v>71</v>
       </c>
@@ -5227,7 +5226,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:12" ht="20.25" customHeight="1">
       <c r="A33" s="22" t="s">
         <v>73</v>
       </c>
@@ -5251,7 +5250,7 @@
       <c r="K33" s="23"/>
       <c r="L33" s="23"/>
     </row>
-    <row r="34" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:12" ht="20.25" customHeight="1">
       <c r="A34" s="22" t="s">
         <v>73</v>
       </c>
@@ -5283,7 +5282,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:12" ht="20.25" customHeight="1">
       <c r="A35" s="22" t="s">
         <v>73</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:12" ht="20.25" customHeight="1">
       <c r="A36" s="22" t="s">
         <v>73</v>
       </c>
@@ -5347,7 +5346,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:12" ht="20.25" customHeight="1">
       <c r="A37" s="22" t="s">
         <v>73</v>
       </c>
@@ -5379,7 +5378,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:12" ht="20.25" customHeight="1">
       <c r="A38" s="22" t="s">
         <v>73</v>
       </c>
@@ -5411,7 +5410,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:12" ht="20.25" customHeight="1">
       <c r="A39" s="22" t="s">
         <v>73</v>
       </c>
@@ -5443,7 +5442,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:12" ht="20.25" customHeight="1">
       <c r="A40" s="22" t="s">
         <v>73</v>
       </c>
@@ -5475,7 +5474,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:12" ht="20.25" customHeight="1">
       <c r="A41" s="22" t="s">
         <v>89</v>
       </c>
@@ -5499,7 +5498,7 @@
       <c r="K41" s="23"/>
       <c r="L41" s="23"/>
     </row>
-    <row r="42" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:12" ht="20.25" customHeight="1">
       <c r="A42" s="22" t="s">
         <v>89</v>
       </c>
@@ -5531,7 +5530,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:12" ht="20.25" customHeight="1">
       <c r="A43" s="22" t="s">
         <v>89</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:12" ht="20.25" customHeight="1">
       <c r="A44" s="22" t="s">
         <v>95</v>
       </c>
@@ -5609,7 +5608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5622,17 +5621,17 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="25" customWidth="1"/>
     <col min="3" max="3" width="58" style="25" customWidth="1"/>
-    <col min="4" max="4" width="133.5" style="25" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="25" customWidth="1"/>
-    <col min="6" max="16384" width="16.33203125" style="25"/>
+    <col min="4" max="4" width="133.42578125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>399</v>
       </c>
@@ -5644,7 +5643,7 @@
       </c>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>402</v>
       </c>
@@ -5658,7 +5657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="32.25" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>405</v>
       </c>
@@ -5672,7 +5671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="32.25" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>407</v>
       </c>
@@ -5686,7 +5685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="32.25" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>410</v>
       </c>
@@ -5700,7 +5699,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="44.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>412</v>
       </c>
@@ -5714,7 +5713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="32.25" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>414</v>
       </c>
@@ -5728,7 +5727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="44.25" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>417</v>
       </c>
@@ -5742,7 +5741,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="32.25" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>420</v>
       </c>
@@ -5756,7 +5755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="32.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>422</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="32.25" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>423</v>
       </c>
@@ -5782,7 +5781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="32.25" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>426</v>
       </c>
@@ -5796,7 +5795,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="32.25" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>429</v>
       </c>
@@ -5810,7 +5809,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="56.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>431</v>
       </c>
@@ -5824,7 +5823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="32.25" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>433</v>
       </c>
@@ -5838,7 +5837,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="32.25" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>436</v>
       </c>
@@ -5852,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="32.25" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>438</v>
       </c>
@@ -5866,7 +5865,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="32.25" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>441</v>
       </c>
@@ -5880,7 +5879,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="32.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>444</v>
       </c>
@@ -5894,7 +5893,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="32.25" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>446</v>
       </c>
@@ -5908,7 +5907,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="56.25" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>449</v>
       </c>
@@ -5922,7 +5921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="44.25" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>451</v>
       </c>
@@ -5936,7 +5935,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="32.25" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>453</v>
       </c>
@@ -5950,7 +5949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>455</v>
       </c>
@@ -5964,7 +5963,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="32.25" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>459</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="44.25" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>461</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="32.25" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>463</v>
       </c>
@@ -6006,7 +6005,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="32.25" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>466</v>
       </c>
@@ -6020,7 +6019,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="32.25" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>468</v>
       </c>
@@ -6034,7 +6033,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="44.25" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>471</v>
       </c>
@@ -6048,7 +6047,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="20.25" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>474</v>
       </c>
@@ -6062,7 +6061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="32.25" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>477</v>
       </c>
@@ -6076,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="44.25" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>480</v>
       </c>
@@ -6090,7 +6089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="32.25" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>482</v>
       </c>
@@ -6104,7 +6103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="32.25" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>485</v>
       </c>
@@ -6118,7 +6117,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="20.25" customHeight="1">
       <c r="A36" s="10" t="s">
         <v>487</v>
       </c>
@@ -6126,7 +6125,7 @@
       <c r="C36" s="34"/>
       <c r="D36" s="34"/>
     </row>
-    <row r="37" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="20.25" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>488</v>
       </c>
@@ -6134,7 +6133,7 @@
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
     </row>
-    <row r="38" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="20.25" customHeight="1">
       <c r="A38" s="10" t="s">
         <v>489</v>
       </c>
@@ -6146,7 +6145,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="20.25" customHeight="1">
       <c r="A39" s="10" t="s">
         <v>492</v>
       </c>
@@ -6154,7 +6153,7 @@
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
     </row>
-    <row r="40" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="32.25" customHeight="1">
       <c r="A40" s="10" t="s">
         <v>493</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="20.25" customHeight="1">
       <c r="A41" s="10" t="s">
         <v>495</v>
       </c>
@@ -6176,7 +6175,7 @@
       </c>
       <c r="D41" s="37"/>
     </row>
-    <row r="42" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="20.25" customHeight="1">
       <c r="A42" s="10" t="s">
         <v>497</v>
       </c>
@@ -6184,7 +6183,7 @@
       <c r="C42" s="34"/>
       <c r="D42" s="34"/>
     </row>
-    <row r="43" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="20.25" customHeight="1">
       <c r="A43" s="10" t="s">
         <v>498</v>
       </c>
@@ -6202,7 +6201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6212,20 +6211,20 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="38" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="38" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="38.5" style="38" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="16.33203125" style="38"/>
+    <col min="1" max="1" width="22.42578125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="38" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>400</v>
       </c>
@@ -6239,7 +6238,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>403</v>
       </c>
@@ -6253,7 +6252,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="20.25" customHeight="1">
       <c r="A3" s="41" t="s">
         <v>403</v>
       </c>
@@ -6267,7 +6266,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
       <c r="A4" s="41" t="s">
         <v>403</v>
       </c>
@@ -6281,7 +6280,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
       <c r="A5" s="41" t="s">
         <v>403</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>512</v>
       </c>
@@ -6309,7 +6308,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
       <c r="A7" s="41" t="s">
         <v>512</v>
       </c>
@@ -6323,7 +6322,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
       <c r="A8" s="41" t="s">
         <v>512</v>
       </c>
@@ -6337,7 +6336,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
       <c r="A9" s="41" t="s">
         <v>512</v>
       </c>
@@ -6351,7 +6350,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>408</v>
       </c>
@@ -6365,7 +6364,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
       <c r="A11" s="41" t="s">
         <v>408</v>
       </c>
@@ -6379,7 +6378,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
       <c r="A12" s="41" t="s">
         <v>408</v>
       </c>
@@ -6393,7 +6392,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
       <c r="A13" s="41" t="s">
         <v>408</v>
       </c>
@@ -6407,7 +6406,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>525</v>
       </c>
@@ -6421,7 +6420,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="20.25" customHeight="1">
       <c r="A15" s="41" t="s">
         <v>525</v>
       </c>
@@ -6435,7 +6434,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="20.25" customHeight="1">
       <c r="A16" s="41" t="s">
         <v>525</v>
       </c>
@@ -6449,35 +6448,35 @@
         <v>528</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="20.25" customHeight="1">
       <c r="A17" s="41" t="s">
         <v>525</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>506</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1">
       <c r="A18" s="41" t="s">
         <v>525</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>456</v>
       </c>
@@ -6488,10 +6487,10 @@
         <v>503</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20.25" customHeight="1">
       <c r="A20" s="41" t="s">
         <v>456</v>
       </c>
@@ -6502,10 +6501,10 @@
         <v>506</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20.25" customHeight="1">
       <c r="A21" s="41" t="s">
         <v>456</v>
       </c>
@@ -6516,49 +6515,49 @@
         <v>506</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20.25" customHeight="1">
       <c r="A22" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C22" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1">
       <c r="A23" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C23" s="42" t="s">
         <v>506</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
       <c r="A24" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C24" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major updates for canada-srm_v1p1
Major updates to prepare for iniital run of canada-srm_va.1
</commit_message>
<xml_diff>
--- a/model-scripts/model-parameters_.xlsx
+++ b/model-scripts/model-parameters_.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/murrayjourneay/OpenDRR/canada-srm2/model-scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjournea\OpenDRR\canada-srm2\model-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1D5FBB-D893-4E43-9930-BA937633A851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="46480" windowHeight="22180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="46485" windowHeight="22185" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="srm-regions" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="srm-parameters" sheetId="3" r:id="rId3"/>
     <sheet name="srm-exports" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1622,12 +1621,6 @@
     <t>eD_[region]_sources.csv</t>
   </si>
   <si>
-    <t>dmg_by_asset</t>
-  </si>
-  <si>
-    <t>eD_[region]_dmg_by_asset_[b0,r2].csv</t>
-  </si>
-  <si>
     <t>consequences.py</t>
   </si>
   <si>
@@ -1659,13 +1652,19 @@
   </si>
   <si>
     <t>ebR_[region]_agg_losses-stats_[b0,r2].csv</t>
+  </si>
+  <si>
+    <t>eD_[region]_damages-meant_[b0,r2].csv</t>
+  </si>
+  <si>
+    <t>avg-damages-mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -3146,7 +3145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3156,21 +3155,21 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="102" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="16.33203125" style="1"/>
+    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3196,7 +3195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="20.25" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="20.25" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -3274,7 +3273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="20.25" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -3300,7 +3299,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="20.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="20.25" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="20.25" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -3378,7 +3377,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="20.25" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
@@ -3404,7 +3403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="20.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
@@ -3430,7 +3429,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="20.25" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="20.25" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
@@ -3482,7 +3481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="20.25" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="20.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
@@ -3534,7 +3533,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="20.25" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="20.25" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
@@ -3586,7 +3585,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="20.25" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>47</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="20.25" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>49</v>
       </c>
@@ -3638,7 +3637,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="20.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>51</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="20.25" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>51</v>
       </c>
@@ -3690,7 +3689,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" ht="20.25" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>51</v>
       </c>
@@ -3716,7 +3715,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="20.25" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>51</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="20.25" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>51</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="20.25" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>51</v>
       </c>
@@ -3794,7 +3793,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="20.25" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>51</v>
       </c>
@@ -3820,7 +3819,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="20.25" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" ht="20.25" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="20.25" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>71</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="20.25" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>73</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="20.25" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>73</v>
       </c>
@@ -3950,7 +3949,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="20.25" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>73</v>
       </c>
@@ -3976,7 +3975,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="20.25" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>73</v>
       </c>
@@ -4002,7 +4001,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="20.25" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>73</v>
       </c>
@@ -4028,7 +4027,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="20.25" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>73</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="20.25" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>73</v>
       </c>
@@ -4080,7 +4079,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" ht="20.25" customHeight="1">
       <c r="A36" s="10" t="s">
         <v>89</v>
       </c>
@@ -4106,7 +4105,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" ht="20.25" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>89</v>
       </c>
@@ -4132,7 +4131,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="20.25" customHeight="1">
       <c r="A38" s="10" t="s">
         <v>95</v>
       </c>
@@ -4168,7 +4167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4178,22 +4177,22 @@
       <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="14.33203125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="19" customWidth="1"/>
+    <col min="1" max="2" width="14.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="19" customWidth="1"/>
     <col min="4" max="4" width="15" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="19" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="19" customWidth="1"/>
     <col min="8" max="8" width="25" style="19" customWidth="1"/>
     <col min="9" max="10" width="29" style="19" customWidth="1"/>
-    <col min="11" max="12" width="25.83203125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="19" customWidth="1"/>
-    <col min="14" max="16384" width="16.33203125" style="19"/>
+    <col min="11" max="12" width="25.85546875" style="19" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="19" customWidth="1"/>
+    <col min="14" max="16384" width="16.28515625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="20.45" customHeight="1">
       <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4254,7 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
     </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="20.25" customHeight="1">
       <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="20.25" customHeight="1">
       <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="20.25" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="A6" s="22" t="s">
         <v>8</v>
       </c>
@@ -4383,7 +4382,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="20.25" customHeight="1">
       <c r="A7" s="22" t="s">
         <v>8</v>
       </c>
@@ -4415,7 +4414,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="20.25" customHeight="1">
       <c r="A8" s="22" t="s">
         <v>20</v>
       </c>
@@ -4441,7 +4440,7 @@
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
     </row>
-    <row r="9" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="20.25" customHeight="1">
       <c r="A9" s="22" t="s">
         <v>20</v>
       </c>
@@ -4475,7 +4474,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="20.25" customHeight="1">
       <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
@@ -4509,7 +4508,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="20.25" customHeight="1">
       <c r="A11" s="22" t="s">
         <v>20</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="20.25" customHeight="1">
       <c r="A12" s="22" t="s">
         <v>20</v>
       </c>
@@ -4577,7 +4576,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="20.25" customHeight="1">
       <c r="A13" s="22" t="s">
         <v>20</v>
       </c>
@@ -4611,7 +4610,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="20.25" customHeight="1">
       <c r="A14" s="22" t="s">
         <v>32</v>
       </c>
@@ -4635,7 +4634,7 @@
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
     </row>
-    <row r="15" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="20.25" customHeight="1">
       <c r="A15" s="22" t="s">
         <v>32</v>
       </c>
@@ -4667,7 +4666,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="20.25" customHeight="1">
       <c r="A16" s="22" t="s">
         <v>32</v>
       </c>
@@ -4699,7 +4698,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="20.25" customHeight="1">
       <c r="A17" s="22" t="s">
         <v>38</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="20.25" customHeight="1">
       <c r="A18" s="22" t="s">
         <v>41</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="20.25" customHeight="1">
       <c r="A19" s="22" t="s">
         <v>44</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="20.25" customHeight="1">
       <c r="A20" s="22" t="s">
         <v>47</v>
       </c>
@@ -4843,7 +4842,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" ht="20.25" customHeight="1">
       <c r="A21" s="22" t="s">
         <v>49</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" ht="20.25" customHeight="1">
       <c r="A22" s="22" t="s">
         <v>51</v>
       </c>
@@ -4903,7 +4902,7 @@
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
     </row>
-    <row r="23" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" ht="20.25" customHeight="1">
       <c r="A23" s="22" t="s">
         <v>51</v>
       </c>
@@ -4935,7 +4934,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" ht="20.25" customHeight="1">
       <c r="A24" s="22" t="s">
         <v>51</v>
       </c>
@@ -4967,7 +4966,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" ht="20.25" customHeight="1">
       <c r="A25" s="22" t="s">
         <v>51</v>
       </c>
@@ -4999,7 +4998,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" ht="20.25" customHeight="1">
       <c r="A26" s="22" t="s">
         <v>51</v>
       </c>
@@ -5031,7 +5030,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" ht="20.25" customHeight="1">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" ht="20.25" customHeight="1">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" ht="20.25" customHeight="1">
       <c r="A29" s="22" t="s">
         <v>51</v>
       </c>
@@ -5127,7 +5126,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" ht="20.25" customHeight="1">
       <c r="A30" s="22" t="s">
         <v>51</v>
       </c>
@@ -5159,7 +5158,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" ht="20.25" customHeight="1">
       <c r="A31" s="22" t="s">
         <v>51</v>
       </c>
@@ -5191,7 +5190,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" ht="20.25" customHeight="1">
       <c r="A32" s="22" t="s">
         <v>71</v>
       </c>
@@ -5227,7 +5226,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:12" ht="20.25" customHeight="1">
       <c r="A33" s="22" t="s">
         <v>73</v>
       </c>
@@ -5251,7 +5250,7 @@
       <c r="K33" s="23"/>
       <c r="L33" s="23"/>
     </row>
-    <row r="34" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:12" ht="20.25" customHeight="1">
       <c r="A34" s="22" t="s">
         <v>73</v>
       </c>
@@ -5283,7 +5282,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:12" ht="20.25" customHeight="1">
       <c r="A35" s="22" t="s">
         <v>73</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:12" ht="20.25" customHeight="1">
       <c r="A36" s="22" t="s">
         <v>73</v>
       </c>
@@ -5347,7 +5346,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:12" ht="20.25" customHeight="1">
       <c r="A37" s="22" t="s">
         <v>73</v>
       </c>
@@ -5379,7 +5378,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:12" ht="20.25" customHeight="1">
       <c r="A38" s="22" t="s">
         <v>73</v>
       </c>
@@ -5411,7 +5410,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:12" ht="20.25" customHeight="1">
       <c r="A39" s="22" t="s">
         <v>73</v>
       </c>
@@ -5443,7 +5442,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:12" ht="20.25" customHeight="1">
       <c r="A40" s="22" t="s">
         <v>73</v>
       </c>
@@ -5475,7 +5474,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:12" ht="20.25" customHeight="1">
       <c r="A41" s="22" t="s">
         <v>89</v>
       </c>
@@ -5499,7 +5498,7 @@
       <c r="K41" s="23"/>
       <c r="L41" s="23"/>
     </row>
-    <row r="42" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:12" ht="20.25" customHeight="1">
       <c r="A42" s="22" t="s">
         <v>89</v>
       </c>
@@ -5531,7 +5530,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:12" ht="20.25" customHeight="1">
       <c r="A43" s="22" t="s">
         <v>89</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:12" ht="20.25" customHeight="1">
       <c r="A44" s="22" t="s">
         <v>95</v>
       </c>
@@ -5609,7 +5608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5622,17 +5621,17 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="25" customWidth="1"/>
     <col min="3" max="3" width="58" style="25" customWidth="1"/>
-    <col min="4" max="4" width="133.5" style="25" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="25" customWidth="1"/>
-    <col min="6" max="16384" width="16.33203125" style="25"/>
+    <col min="4" max="4" width="133.42578125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>399</v>
       </c>
@@ -5644,7 +5643,7 @@
       </c>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>402</v>
       </c>
@@ -5658,7 +5657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="32.25" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>405</v>
       </c>
@@ -5672,7 +5671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="32.25" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>407</v>
       </c>
@@ -5686,7 +5685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="32.25" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>410</v>
       </c>
@@ -5700,7 +5699,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="44.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>412</v>
       </c>
@@ -5714,7 +5713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="32.25" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>414</v>
       </c>
@@ -5728,7 +5727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="44.25" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>417</v>
       </c>
@@ -5742,7 +5741,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="32.25" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>420</v>
       </c>
@@ -5756,7 +5755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="32.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>422</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="32.25" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>423</v>
       </c>
@@ -5782,7 +5781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="32.25" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>426</v>
       </c>
@@ -5796,7 +5795,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="32.25" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>429</v>
       </c>
@@ -5810,7 +5809,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="56.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>431</v>
       </c>
@@ -5824,7 +5823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="32.25" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>433</v>
       </c>
@@ -5838,7 +5837,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="32.25" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>436</v>
       </c>
@@ -5852,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="32.25" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>438</v>
       </c>
@@ -5866,7 +5865,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="32.25" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>441</v>
       </c>
@@ -5880,7 +5879,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="32.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>444</v>
       </c>
@@ -5894,7 +5893,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="32.25" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>446</v>
       </c>
@@ -5908,7 +5907,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="56.25" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>449</v>
       </c>
@@ -5922,7 +5921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="44.25" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>451</v>
       </c>
@@ -5936,7 +5935,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="32.25" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>453</v>
       </c>
@@ -5950,7 +5949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>455</v>
       </c>
@@ -5964,7 +5963,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="32.25" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>459</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="44.25" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>461</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="32.25" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>463</v>
       </c>
@@ -6006,7 +6005,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="32.25" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>466</v>
       </c>
@@ -6020,7 +6019,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="32.25" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>468</v>
       </c>
@@ -6034,7 +6033,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="44.25" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>471</v>
       </c>
@@ -6048,7 +6047,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="20.25" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>474</v>
       </c>
@@ -6062,7 +6061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="32.25" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>477</v>
       </c>
@@ -6076,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="44.25" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>480</v>
       </c>
@@ -6090,7 +6089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="32.25" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>482</v>
       </c>
@@ -6104,7 +6103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="32.25" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>485</v>
       </c>
@@ -6118,7 +6117,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="20.25" customHeight="1">
       <c r="A36" s="10" t="s">
         <v>487</v>
       </c>
@@ -6126,7 +6125,7 @@
       <c r="C36" s="34"/>
       <c r="D36" s="34"/>
     </row>
-    <row r="37" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="20.25" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>488</v>
       </c>
@@ -6134,7 +6133,7 @@
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
     </row>
-    <row r="38" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="20.25" customHeight="1">
       <c r="A38" s="10" t="s">
         <v>489</v>
       </c>
@@ -6146,7 +6145,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="20.25" customHeight="1">
       <c r="A39" s="10" t="s">
         <v>492</v>
       </c>
@@ -6154,7 +6153,7 @@
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
     </row>
-    <row r="40" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="32.25" customHeight="1">
       <c r="A40" s="10" t="s">
         <v>493</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="20.25" customHeight="1">
       <c r="A41" s="10" t="s">
         <v>495</v>
       </c>
@@ -6176,7 +6175,7 @@
       </c>
       <c r="D41" s="37"/>
     </row>
-    <row r="42" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="20.25" customHeight="1">
       <c r="A42" s="10" t="s">
         <v>497</v>
       </c>
@@ -6184,7 +6183,7 @@
       <c r="C42" s="34"/>
       <c r="D42" s="34"/>
     </row>
-    <row r="43" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="20.25" customHeight="1">
       <c r="A43" s="10" t="s">
         <v>498</v>
       </c>
@@ -6202,7 +6201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6212,20 +6211,20 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="38" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="38" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="38.5" style="38" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="16.33203125" style="38"/>
+    <col min="1" max="1" width="22.42578125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="38" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>400</v>
       </c>
@@ -6239,7 +6238,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>403</v>
       </c>
@@ -6253,7 +6252,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="20.25" customHeight="1">
       <c r="A3" s="41" t="s">
         <v>403</v>
       </c>
@@ -6267,7 +6266,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
       <c r="A4" s="41" t="s">
         <v>403</v>
       </c>
@@ -6281,7 +6280,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
       <c r="A5" s="41" t="s">
         <v>403</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>512</v>
       </c>
@@ -6309,7 +6308,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
       <c r="A7" s="41" t="s">
         <v>512</v>
       </c>
@@ -6323,7 +6322,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
       <c r="A8" s="41" t="s">
         <v>512</v>
       </c>
@@ -6337,7 +6336,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
       <c r="A9" s="41" t="s">
         <v>512</v>
       </c>
@@ -6351,7 +6350,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>408</v>
       </c>
@@ -6365,7 +6364,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
       <c r="A11" s="41" t="s">
         <v>408</v>
       </c>
@@ -6379,7 +6378,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
       <c r="A12" s="41" t="s">
         <v>408</v>
       </c>
@@ -6393,7 +6392,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
       <c r="A13" s="41" t="s">
         <v>408</v>
       </c>
@@ -6407,7 +6406,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>525</v>
       </c>
@@ -6421,7 +6420,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="20.25" customHeight="1">
       <c r="A15" s="41" t="s">
         <v>525</v>
       </c>
@@ -6435,7 +6434,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="20.25" customHeight="1">
       <c r="A16" s="41" t="s">
         <v>525</v>
       </c>
@@ -6449,35 +6448,35 @@
         <v>528</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="20.25" customHeight="1">
       <c r="A17" s="41" t="s">
         <v>525</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>506</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1">
       <c r="A18" s="41" t="s">
         <v>525</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>456</v>
       </c>
@@ -6488,10 +6487,10 @@
         <v>503</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20.25" customHeight="1">
       <c r="A20" s="41" t="s">
         <v>456</v>
       </c>
@@ -6502,10 +6501,10 @@
         <v>506</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20.25" customHeight="1">
       <c r="A21" s="41" t="s">
         <v>456</v>
       </c>
@@ -6516,49 +6515,49 @@
         <v>506</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20.25" customHeight="1">
       <c r="A22" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C22" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1">
       <c r="A23" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C23" s="42" t="s">
         <v>506</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
       <c r="A24" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C24" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major updates for canada-srm_v1p1 (#10)
Major updates to prepare for iniital run of canada-srm_va.1
</commit_message>
<xml_diff>
--- a/model-scripts/model-parameters_.xlsx
+++ b/model-scripts/model-parameters_.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/murrayjourneay/OpenDRR/canada-srm2/model-scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjournea\OpenDRR\canada-srm2\model-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1D5FBB-D893-4E43-9930-BA937633A851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="46480" windowHeight="22180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="46485" windowHeight="22185" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="srm-regions" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="srm-parameters" sheetId="3" r:id="rId3"/>
     <sheet name="srm-exports" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1622,12 +1621,6 @@
     <t>eD_[region]_sources.csv</t>
   </si>
   <si>
-    <t>dmg_by_asset</t>
-  </si>
-  <si>
-    <t>eD_[region]_dmg_by_asset_[b0,r2].csv</t>
-  </si>
-  <si>
     <t>consequences.py</t>
   </si>
   <si>
@@ -1659,13 +1652,19 @@
   </si>
   <si>
     <t>ebR_[region]_agg_losses-stats_[b0,r2].csv</t>
+  </si>
+  <si>
+    <t>eD_[region]_damages-meant_[b0,r2].csv</t>
+  </si>
+  <si>
+    <t>avg-damages-mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -3146,7 +3145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3156,21 +3155,21 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="102" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="16.33203125" style="1"/>
+    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3196,7 +3195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="20.25" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="20.25" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -3274,7 +3273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="20.25" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -3300,7 +3299,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="20.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="20.25" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="20.25" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -3378,7 +3377,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="20.25" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
@@ -3404,7 +3403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="20.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
@@ -3430,7 +3429,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="20.25" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="20.25" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
@@ -3482,7 +3481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="20.25" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="20.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
@@ -3534,7 +3533,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="20.25" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="20.25" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
@@ -3586,7 +3585,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="20.25" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>47</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="20.25" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>49</v>
       </c>
@@ -3638,7 +3637,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="20.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>51</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="20.25" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>51</v>
       </c>
@@ -3690,7 +3689,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" ht="20.25" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>51</v>
       </c>
@@ -3716,7 +3715,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="20.25" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>51</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="20.25" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>51</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="20.25" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>51</v>
       </c>
@@ -3794,7 +3793,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="20.25" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>51</v>
       </c>
@@ -3820,7 +3819,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="20.25" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" ht="20.25" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="20.25" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>71</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="20.25" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>73</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="20.25" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>73</v>
       </c>
@@ -3950,7 +3949,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="20.25" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>73</v>
       </c>
@@ -3976,7 +3975,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="20.25" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>73</v>
       </c>
@@ -4002,7 +4001,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="20.25" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>73</v>
       </c>
@@ -4028,7 +4027,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="20.25" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>73</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="20.25" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>73</v>
       </c>
@@ -4080,7 +4079,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" ht="20.25" customHeight="1">
       <c r="A36" s="10" t="s">
         <v>89</v>
       </c>
@@ -4106,7 +4105,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" ht="20.25" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>89</v>
       </c>
@@ -4132,7 +4131,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="20.25" customHeight="1">
       <c r="A38" s="10" t="s">
         <v>95</v>
       </c>
@@ -4168,7 +4167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4178,22 +4177,22 @@
       <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="14.33203125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="19" customWidth="1"/>
+    <col min="1" max="2" width="14.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="19" customWidth="1"/>
     <col min="4" max="4" width="15" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="19" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="19" customWidth="1"/>
     <col min="8" max="8" width="25" style="19" customWidth="1"/>
     <col min="9" max="10" width="29" style="19" customWidth="1"/>
-    <col min="11" max="12" width="25.83203125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="19" customWidth="1"/>
-    <col min="14" max="16384" width="16.33203125" style="19"/>
+    <col min="11" max="12" width="25.85546875" style="19" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="19" customWidth="1"/>
+    <col min="14" max="16384" width="16.28515625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="20.45" customHeight="1">
       <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4254,7 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
     </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="20.25" customHeight="1">
       <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="20.25" customHeight="1">
       <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="20.25" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="A6" s="22" t="s">
         <v>8</v>
       </c>
@@ -4383,7 +4382,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="20.25" customHeight="1">
       <c r="A7" s="22" t="s">
         <v>8</v>
       </c>
@@ -4415,7 +4414,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="20.25" customHeight="1">
       <c r="A8" s="22" t="s">
         <v>20</v>
       </c>
@@ -4441,7 +4440,7 @@
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
     </row>
-    <row r="9" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="20.25" customHeight="1">
       <c r="A9" s="22" t="s">
         <v>20</v>
       </c>
@@ -4475,7 +4474,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="20.25" customHeight="1">
       <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
@@ -4509,7 +4508,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="20.25" customHeight="1">
       <c r="A11" s="22" t="s">
         <v>20</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="20.25" customHeight="1">
       <c r="A12" s="22" t="s">
         <v>20</v>
       </c>
@@ -4577,7 +4576,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="20.25" customHeight="1">
       <c r="A13" s="22" t="s">
         <v>20</v>
       </c>
@@ -4611,7 +4610,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="20.25" customHeight="1">
       <c r="A14" s="22" t="s">
         <v>32</v>
       </c>
@@ -4635,7 +4634,7 @@
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
     </row>
-    <row r="15" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="20.25" customHeight="1">
       <c r="A15" s="22" t="s">
         <v>32</v>
       </c>
@@ -4667,7 +4666,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="20.25" customHeight="1">
       <c r="A16" s="22" t="s">
         <v>32</v>
       </c>
@@ -4699,7 +4698,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="20.25" customHeight="1">
       <c r="A17" s="22" t="s">
         <v>38</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="20.25" customHeight="1">
       <c r="A18" s="22" t="s">
         <v>41</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="20.25" customHeight="1">
       <c r="A19" s="22" t="s">
         <v>44</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="20.25" customHeight="1">
       <c r="A20" s="22" t="s">
         <v>47</v>
       </c>
@@ -4843,7 +4842,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" ht="20.25" customHeight="1">
       <c r="A21" s="22" t="s">
         <v>49</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" ht="20.25" customHeight="1">
       <c r="A22" s="22" t="s">
         <v>51</v>
       </c>
@@ -4903,7 +4902,7 @@
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
     </row>
-    <row r="23" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" ht="20.25" customHeight="1">
       <c r="A23" s="22" t="s">
         <v>51</v>
       </c>
@@ -4935,7 +4934,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" ht="20.25" customHeight="1">
       <c r="A24" s="22" t="s">
         <v>51</v>
       </c>
@@ -4967,7 +4966,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" ht="20.25" customHeight="1">
       <c r="A25" s="22" t="s">
         <v>51</v>
       </c>
@@ -4999,7 +4998,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" ht="20.25" customHeight="1">
       <c r="A26" s="22" t="s">
         <v>51</v>
       </c>
@@ -5031,7 +5030,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" ht="20.25" customHeight="1">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" ht="20.25" customHeight="1">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" ht="20.25" customHeight="1">
       <c r="A29" s="22" t="s">
         <v>51</v>
       </c>
@@ -5127,7 +5126,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" ht="20.25" customHeight="1">
       <c r="A30" s="22" t="s">
         <v>51</v>
       </c>
@@ -5159,7 +5158,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" ht="20.25" customHeight="1">
       <c r="A31" s="22" t="s">
         <v>51</v>
       </c>
@@ -5191,7 +5190,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" ht="20.25" customHeight="1">
       <c r="A32" s="22" t="s">
         <v>71</v>
       </c>
@@ -5227,7 +5226,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:12" ht="20.25" customHeight="1">
       <c r="A33" s="22" t="s">
         <v>73</v>
       </c>
@@ -5251,7 +5250,7 @@
       <c r="K33" s="23"/>
       <c r="L33" s="23"/>
     </row>
-    <row r="34" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:12" ht="20.25" customHeight="1">
       <c r="A34" s="22" t="s">
         <v>73</v>
       </c>
@@ -5283,7 +5282,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:12" ht="20.25" customHeight="1">
       <c r="A35" s="22" t="s">
         <v>73</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:12" ht="20.25" customHeight="1">
       <c r="A36" s="22" t="s">
         <v>73</v>
       </c>
@@ -5347,7 +5346,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:12" ht="20.25" customHeight="1">
       <c r="A37" s="22" t="s">
         <v>73</v>
       </c>
@@ -5379,7 +5378,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:12" ht="20.25" customHeight="1">
       <c r="A38" s="22" t="s">
         <v>73</v>
       </c>
@@ -5411,7 +5410,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:12" ht="20.25" customHeight="1">
       <c r="A39" s="22" t="s">
         <v>73</v>
       </c>
@@ -5443,7 +5442,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:12" ht="20.25" customHeight="1">
       <c r="A40" s="22" t="s">
         <v>73</v>
       </c>
@@ -5475,7 +5474,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:12" ht="20.25" customHeight="1">
       <c r="A41" s="22" t="s">
         <v>89</v>
       </c>
@@ -5499,7 +5498,7 @@
       <c r="K41" s="23"/>
       <c r="L41" s="23"/>
     </row>
-    <row r="42" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:12" ht="20.25" customHeight="1">
       <c r="A42" s="22" t="s">
         <v>89</v>
       </c>
@@ -5531,7 +5530,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:12" ht="20.25" customHeight="1">
       <c r="A43" s="22" t="s">
         <v>89</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:12" ht="20.25" customHeight="1">
       <c r="A44" s="22" t="s">
         <v>95</v>
       </c>
@@ -5609,7 +5608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5622,17 +5621,17 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="25" customWidth="1"/>
     <col min="3" max="3" width="58" style="25" customWidth="1"/>
-    <col min="4" max="4" width="133.5" style="25" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="25" customWidth="1"/>
-    <col min="6" max="16384" width="16.33203125" style="25"/>
+    <col min="4" max="4" width="133.42578125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>399</v>
       </c>
@@ -5644,7 +5643,7 @@
       </c>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>402</v>
       </c>
@@ -5658,7 +5657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="32.25" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>405</v>
       </c>
@@ -5672,7 +5671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="32.25" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>407</v>
       </c>
@@ -5686,7 +5685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="32.25" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>410</v>
       </c>
@@ -5700,7 +5699,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="44.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>412</v>
       </c>
@@ -5714,7 +5713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="32.25" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>414</v>
       </c>
@@ -5728,7 +5727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="44.25" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>417</v>
       </c>
@@ -5742,7 +5741,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="32.25" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>420</v>
       </c>
@@ -5756,7 +5755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="32.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>422</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="32.25" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>423</v>
       </c>
@@ -5782,7 +5781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="32.25" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>426</v>
       </c>
@@ -5796,7 +5795,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="32.25" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>429</v>
       </c>
@@ -5810,7 +5809,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="56.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>431</v>
       </c>
@@ -5824,7 +5823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="32.25" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>433</v>
       </c>
@@ -5838,7 +5837,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="32.25" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>436</v>
       </c>
@@ -5852,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="32.25" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>438</v>
       </c>
@@ -5866,7 +5865,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="32.25" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>441</v>
       </c>
@@ -5880,7 +5879,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="32.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>444</v>
       </c>
@@ -5894,7 +5893,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="32.25" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>446</v>
       </c>
@@ -5908,7 +5907,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="56.25" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>449</v>
       </c>
@@ -5922,7 +5921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="44.25" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>451</v>
       </c>
@@ -5936,7 +5935,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="32.25" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>453</v>
       </c>
@@ -5950,7 +5949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>455</v>
       </c>
@@ -5964,7 +5963,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="32.25" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>459</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="44.25" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>461</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="32.25" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>463</v>
       </c>
@@ -6006,7 +6005,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="32.25" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>466</v>
       </c>
@@ -6020,7 +6019,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="32.25" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>468</v>
       </c>
@@ -6034,7 +6033,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="44.25" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>471</v>
       </c>
@@ -6048,7 +6047,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="20.25" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>474</v>
       </c>
@@ -6062,7 +6061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="32.25" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>477</v>
       </c>
@@ -6076,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="44.25" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>480</v>
       </c>
@@ -6090,7 +6089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="32.25" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>482</v>
       </c>
@@ -6104,7 +6103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="32.25" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>485</v>
       </c>
@@ -6118,7 +6117,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="20.25" customHeight="1">
       <c r="A36" s="10" t="s">
         <v>487</v>
       </c>
@@ -6126,7 +6125,7 @@
       <c r="C36" s="34"/>
       <c r="D36" s="34"/>
     </row>
-    <row r="37" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="20.25" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>488</v>
       </c>
@@ -6134,7 +6133,7 @@
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
     </row>
-    <row r="38" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="20.25" customHeight="1">
       <c r="A38" s="10" t="s">
         <v>489</v>
       </c>
@@ -6146,7 +6145,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="20.25" customHeight="1">
       <c r="A39" s="10" t="s">
         <v>492</v>
       </c>
@@ -6154,7 +6153,7 @@
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
     </row>
-    <row r="40" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="32.25" customHeight="1">
       <c r="A40" s="10" t="s">
         <v>493</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="20.25" customHeight="1">
       <c r="A41" s="10" t="s">
         <v>495</v>
       </c>
@@ -6176,7 +6175,7 @@
       </c>
       <c r="D41" s="37"/>
     </row>
-    <row r="42" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="20.25" customHeight="1">
       <c r="A42" s="10" t="s">
         <v>497</v>
       </c>
@@ -6184,7 +6183,7 @@
       <c r="C42" s="34"/>
       <c r="D42" s="34"/>
     </row>
-    <row r="43" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="20.25" customHeight="1">
       <c r="A43" s="10" t="s">
         <v>498</v>
       </c>
@@ -6202,7 +6201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6212,20 +6211,20 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="38" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="38" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="38.5" style="38" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="16.33203125" style="38"/>
+    <col min="1" max="1" width="22.42578125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="38" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="20.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>400</v>
       </c>
@@ -6239,7 +6238,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>403</v>
       </c>
@@ -6253,7 +6252,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="20.25" customHeight="1">
       <c r="A3" s="41" t="s">
         <v>403</v>
       </c>
@@ -6267,7 +6266,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
       <c r="A4" s="41" t="s">
         <v>403</v>
       </c>
@@ -6281,7 +6280,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
       <c r="A5" s="41" t="s">
         <v>403</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>512</v>
       </c>
@@ -6309,7 +6308,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
       <c r="A7" s="41" t="s">
         <v>512</v>
       </c>
@@ -6323,7 +6322,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
       <c r="A8" s="41" t="s">
         <v>512</v>
       </c>
@@ -6337,7 +6336,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
       <c r="A9" s="41" t="s">
         <v>512</v>
       </c>
@@ -6351,7 +6350,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>408</v>
       </c>
@@ -6365,7 +6364,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
       <c r="A11" s="41" t="s">
         <v>408</v>
       </c>
@@ -6379,7 +6378,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
       <c r="A12" s="41" t="s">
         <v>408</v>
       </c>
@@ -6393,7 +6392,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
       <c r="A13" s="41" t="s">
         <v>408</v>
       </c>
@@ -6407,7 +6406,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>525</v>
       </c>
@@ -6421,7 +6420,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="20.25" customHeight="1">
       <c r="A15" s="41" t="s">
         <v>525</v>
       </c>
@@ -6435,7 +6434,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="20.25" customHeight="1">
       <c r="A16" s="41" t="s">
         <v>525</v>
       </c>
@@ -6449,35 +6448,35 @@
         <v>528</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="20.25" customHeight="1">
       <c r="A17" s="41" t="s">
         <v>525</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>506</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1">
       <c r="A18" s="41" t="s">
         <v>525</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20.25" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>456</v>
       </c>
@@ -6488,10 +6487,10 @@
         <v>503</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20.25" customHeight="1">
       <c r="A20" s="41" t="s">
         <v>456</v>
       </c>
@@ -6502,10 +6501,10 @@
         <v>506</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20.25" customHeight="1">
       <c r="A21" s="41" t="s">
         <v>456</v>
       </c>
@@ -6516,49 +6515,49 @@
         <v>506</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20.25" customHeight="1">
       <c r="A22" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C22" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1">
       <c r="A23" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C23" s="42" t="s">
         <v>506</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
       <c r="A24" s="41" t="s">
         <v>456</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C24" s="43" t="s">
         <v>506</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>